<commit_message>
switched to petry for package management
</commit_message>
<xml_diff>
--- a/canteen/media/Student/student.xlsx
+++ b/canteen/media/Student/student.xlsx
@@ -31,7 +31,7 @@
     <t>Semester</t>
   </si>
   <si>
-    <t>Sujan Khattri</t>
+    <t>hello khatri</t>
   </si>
   <si>
     <t>college</t>
@@ -438,7 +438,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3">
-        <v>9089089890</v>
+        <v>10101</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>

</xml_diff>